<commit_message>
this is all the Prep
</commit_message>
<xml_diff>
--- a/sample_tables (version 1).xlsb.xlsx
+++ b/sample_tables (version 1).xlsb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danig\Documents\GitHub\Research\DataTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2012436E-01EE-4A78-BD3F-27FE6A1B0EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0DF00D-B38F-4C1A-83EB-6042FC8BB7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="780" yWindow="30" windowWidth="18680" windowHeight="12980" activeTab="7" xr2:uid="{94E6D992-0F2D-4B9D-BD81-1E9E3BDAA891}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="7" xr2:uid="{94E6D992-0F2D-4B9D-BD81-1E9E3BDAA891}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">datasetX_t2!$C$1:$M$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -74,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="74">
   <si>
     <t>Table PNG</t>
   </si>
@@ -289,6 +288,15 @@
   <si>
     <t>k</t>
   </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
 </sst>
 </file>
 
@@ -483,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -601,23 +609,6 @@
     <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -627,6 +618,12 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,9 +643,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -686,7 +683,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -792,7 +789,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -934,7 +931,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -948,19 +945,19 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="93" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1053,7 @@
       <c r="BO1" s="10"/>
       <c r="BP1" s="10"/>
     </row>
-    <row r="2" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="str">
         <f t="shared" ref="A2:A21" si="0">"DS"&amp;C2 &amp;"_"&amp;D2 &amp;"_"&amp;E2 &amp;F2&amp;".png"</f>
         <v>DS0_anime_color1.png</v>
@@ -1143,7 +1140,7 @@
       <c r="BO2" s="18"/>
       <c r="BP2" s="18"/>
     </row>
-    <row r="3" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_zebra2.png</v>
@@ -1230,7 +1227,7 @@
       <c r="BO3" s="18"/>
       <c r="BP3" s="18"/>
     </row>
-    <row r="4" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_plain3.png</v>
@@ -1317,7 +1314,7 @@
       <c r="BO4" s="18"/>
       <c r="BP4" s="18"/>
     </row>
-    <row r="5" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_bar4.png</v>
@@ -1404,7 +1401,7 @@
       <c r="BO5" s="18"/>
       <c r="BP5" s="18"/>
     </row>
-    <row r="6" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="30" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_color1.png</v>
@@ -1445,7 +1442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="30" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_zebra2.png</v>
@@ -1486,7 +1483,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="str">
         <f t="shared" si="0"/>
         <v>DSX_anime_plain3.png</v>
@@ -1528,7 +1525,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="30" t="str">
         <f t="shared" si="0"/>
         <v>DSX_anime_bar4.png</v>
@@ -1570,7 +1567,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="34" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_color1.png</v>
@@ -1651,7 +1648,7 @@
         <v>14 23 29</v>
       </c>
     </row>
-    <row r="11" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="34" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_zebra2.png</v>
@@ -1732,7 +1729,7 @@
         <v>23 15 18</v>
       </c>
     </row>
-    <row r="12" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="34" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_plain3.png</v>
@@ -1813,7 +1810,7 @@
         <v>30 11 13</v>
       </c>
     </row>
-    <row r="13" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="34" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_bar4.png</v>
@@ -1894,7 +1891,7 @@
         <v>15 3 8</v>
       </c>
     </row>
-    <row r="14" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="38" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_color1.png</v>
@@ -1937,7 +1934,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="38" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_zebra2.png</v>
@@ -1978,7 +1975,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_plain3.png</v>
@@ -2019,7 +2016,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" s="38" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="38" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_bar4.png</v>
@@ -2060,7 +2057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_color1.png</v>
@@ -2107,7 +2104,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_zebra2.png</v>
@@ -2154,7 +2151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_plain3.png</v>
@@ -2201,7 +2198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="str">
         <f t="shared" si="0"/>
         <v>DS0_anime_bar4.png</v>
@@ -2261,18 +2258,18 @@
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="45" customWidth="1"/>
-    <col min="4" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="45" customWidth="1"/>
-    <col min="12" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" style="45" customWidth="1"/>
+    <col min="4" max="10" width="16.453125" customWidth="1"/>
+    <col min="11" max="11" width="16.453125" style="45" customWidth="1"/>
+    <col min="12" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="42"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -2286,7 +2283,7 @@
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="37" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="22" t="s">
         <v>28</v>
@@ -2326,7 +2323,7 @@
       </c>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B3" s="23" t="s">
         <v>60</v>
       </c>
@@ -2365,7 +2362,7 @@
       </c>
       <c r="N3" s="19"/>
     </row>
-    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B4" s="23" t="s">
         <v>68</v>
       </c>
@@ -2404,7 +2401,7 @@
       </c>
       <c r="N4" s="19"/>
     </row>
-    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B5" s="23" t="s">
         <v>47</v>
       </c>
@@ -2443,7 +2440,7 @@
       </c>
       <c r="N5" s="19"/>
     </row>
-    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B6" s="23" t="s">
         <v>54</v>
       </c>
@@ -2482,7 +2479,7 @@
       </c>
       <c r="N6" s="19"/>
     </row>
-    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B7" s="23" t="s">
         <v>48</v>
       </c>
@@ -2521,7 +2518,7 @@
       </c>
       <c r="N7" s="19"/>
     </row>
-    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B8" s="23" t="s">
         <v>44</v>
       </c>
@@ -2560,7 +2557,7 @@
       </c>
       <c r="N8" s="19"/>
     </row>
-    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B9" s="23" t="s">
         <v>50</v>
       </c>
@@ -2599,7 +2596,7 @@
       </c>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B10" s="23" t="s">
         <v>58</v>
       </c>
@@ -2638,7 +2635,7 @@
       </c>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B11" s="23" t="s">
         <v>65</v>
       </c>
@@ -2677,7 +2674,7 @@
       </c>
       <c r="N11" s="19"/>
     </row>
-    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B12" s="23" t="s">
         <v>51</v>
       </c>
@@ -2716,7 +2713,7 @@
       </c>
       <c r="N12" s="19"/>
     </row>
-    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B13" s="23" t="s">
         <v>52</v>
       </c>
@@ -2755,7 +2752,7 @@
       </c>
       <c r="N13" s="19"/>
     </row>
-    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B14" s="23" t="s">
         <v>53</v>
       </c>
@@ -2794,7 +2791,7 @@
       </c>
       <c r="N14" s="19"/>
     </row>
-    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B15" s="23" t="s">
         <v>42</v>
       </c>
@@ -2833,7 +2830,7 @@
       </c>
       <c r="N15" s="19"/>
     </row>
-    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B16" s="23" t="s">
         <v>45</v>
       </c>
@@ -2872,7 +2869,7 @@
       </c>
       <c r="N16" s="19"/>
     </row>
-    <row r="17" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B17" s="23" t="s">
         <v>46</v>
       </c>
@@ -2911,7 +2908,7 @@
       </c>
       <c r="N17" s="19"/>
     </row>
-    <row r="18" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B18" s="23" t="s">
         <v>67</v>
       </c>
@@ -2950,7 +2947,7 @@
       </c>
       <c r="N18" s="19"/>
     </row>
-    <row r="19" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B19" s="23" t="s">
         <v>49</v>
       </c>
@@ -2989,7 +2986,7 @@
       </c>
       <c r="N19" s="19"/>
     </row>
-    <row r="20" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B20" s="23" t="s">
         <v>63</v>
       </c>
@@ -3028,7 +3025,7 @@
       </c>
       <c r="N20" s="19"/>
     </row>
-    <row r="21" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B21" s="23" t="s">
         <v>56</v>
       </c>
@@ -3067,7 +3064,7 @@
       </c>
       <c r="N21" s="19"/>
     </row>
-    <row r="22" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B22" s="23" t="s">
         <v>64</v>
       </c>
@@ -3106,7 +3103,7 @@
       </c>
       <c r="N22" s="19"/>
     </row>
-    <row r="23" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B23" s="23" t="s">
         <v>55</v>
       </c>
@@ -3145,7 +3142,7 @@
       </c>
       <c r="N23" s="19"/>
     </row>
-    <row r="24" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B24" s="23" t="s">
         <v>40</v>
       </c>
@@ -3184,7 +3181,7 @@
       </c>
       <c r="N24" s="19"/>
     </row>
-    <row r="25" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B25" s="23" t="s">
         <v>62</v>
       </c>
@@ -3223,7 +3220,7 @@
       </c>
       <c r="N25" s="19"/>
     </row>
-    <row r="26" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B26" s="23" t="s">
         <v>59</v>
       </c>
@@ -3262,7 +3259,7 @@
       </c>
       <c r="N26" s="19"/>
     </row>
-    <row r="27" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B27" s="23" t="s">
         <v>43</v>
       </c>
@@ -3301,7 +3298,7 @@
       </c>
       <c r="N27" s="19"/>
     </row>
-    <row r="28" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B28" s="23" t="s">
         <v>41</v>
       </c>
@@ -3340,7 +3337,7 @@
       </c>
       <c r="N28" s="19"/>
     </row>
-    <row r="29" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B29" s="23" t="s">
         <v>57</v>
       </c>
@@ -3379,7 +3376,7 @@
       </c>
       <c r="N29" s="19"/>
     </row>
-    <row r="30" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B30" s="23" t="s">
         <v>61</v>
       </c>
@@ -3418,7 +3415,7 @@
       </c>
       <c r="N30" s="19"/>
     </row>
-    <row r="31" spans="2:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B31" s="23" t="s">
         <v>66</v>
       </c>
@@ -3457,7 +3454,7 @@
       </c>
       <c r="N31" s="19"/>
     </row>
-    <row r="32" spans="2:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" ht="18.5" x14ac:dyDescent="0.35">
       <c r="B32" s="25"/>
       <c r="C32" s="42"/>
       <c r="D32" s="19"/>
@@ -3597,37 +3594,34 @@
       <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="49" customWidth="1"/>
-    <col min="4" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="49" customWidth="1"/>
-    <col min="10" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="50"/>
+    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
-      <c r="I1" s="50"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="37" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="22" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="22" t="s">
@@ -3645,7 +3639,7 @@
       <c r="H2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="52" t="s">
+      <c r="I2" s="22" t="s">
         <v>38</v>
       </c>
       <c r="J2" s="22" t="s">
@@ -3661,11 +3655,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B3" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="24">
         <v>47</v>
       </c>
       <c r="D3" s="24">
@@ -3683,7 +3677,7 @@
       <c r="H3" s="24">
         <v>25</v>
       </c>
-      <c r="I3" s="54">
+      <c r="I3" s="24">
         <v>53</v>
       </c>
       <c r="J3" s="24">
@@ -3699,11 +3693,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B4" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="24">
         <v>15</v>
       </c>
       <c r="D4" s="24">
@@ -3721,7 +3715,7 @@
       <c r="H4" s="24">
         <v>78</v>
       </c>
-      <c r="I4" s="54">
+      <c r="I4" s="24">
         <v>17</v>
       </c>
       <c r="J4" s="24">
@@ -3737,11 +3731,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B5" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="24">
         <v>17</v>
       </c>
       <c r="D5" s="24">
@@ -3759,7 +3753,7 @@
       <c r="H5" s="24">
         <v>38</v>
       </c>
-      <c r="I5" s="54">
+      <c r="I5" s="24">
         <v>19</v>
       </c>
       <c r="J5" s="24">
@@ -3775,11 +3769,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B6" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="24">
         <v>32</v>
       </c>
       <c r="D6" s="24">
@@ -3797,7 +3791,7 @@
       <c r="H6" s="24">
         <v>41</v>
       </c>
-      <c r="I6" s="54">
+      <c r="I6" s="24">
         <v>36</v>
       </c>
       <c r="J6" s="24">
@@ -3813,11 +3807,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="24">
         <v>31</v>
       </c>
       <c r="D7" s="24">
@@ -3835,7 +3829,7 @@
       <c r="H7" s="24">
         <v>40</v>
       </c>
-      <c r="I7" s="54">
+      <c r="I7" s="24">
         <v>35</v>
       </c>
       <c r="J7" s="24">
@@ -3851,11 +3845,11 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B8" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="24">
         <v>46</v>
       </c>
       <c r="D8" s="24">
@@ -3873,7 +3867,7 @@
       <c r="H8" s="24">
         <v>30</v>
       </c>
-      <c r="I8" s="54">
+      <c r="I8" s="24">
         <v>51</v>
       </c>
       <c r="J8" s="24">
@@ -3889,11 +3883,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B9" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="24">
         <v>36</v>
       </c>
       <c r="D9" s="24">
@@ -3911,7 +3905,7 @@
       <c r="H9" s="24">
         <v>46</v>
       </c>
-      <c r="I9" s="54">
+      <c r="I9" s="24">
         <v>40</v>
       </c>
       <c r="J9" s="24">
@@ -3927,11 +3921,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B10" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="24">
         <v>17</v>
       </c>
       <c r="D10" s="24">
@@ -3949,7 +3943,7 @@
       <c r="H10" s="24">
         <v>41</v>
       </c>
-      <c r="I10" s="54">
+      <c r="I10" s="24">
         <v>19</v>
       </c>
       <c r="J10" s="24">
@@ -3965,11 +3959,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B11" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="24">
         <v>19</v>
       </c>
       <c r="D11" s="24">
@@ -3987,7 +3981,7 @@
       <c r="H11" s="24">
         <v>87</v>
       </c>
-      <c r="I11" s="54">
+      <c r="I11" s="24">
         <v>22</v>
       </c>
       <c r="J11" s="24">
@@ -4003,11 +3997,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B12" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="24">
         <v>25</v>
       </c>
       <c r="D12" s="24">
@@ -4025,7 +4019,7 @@
       <c r="H12" s="24">
         <v>90</v>
       </c>
-      <c r="I12" s="54">
+      <c r="I12" s="24">
         <v>28</v>
       </c>
       <c r="J12" s="24">
@@ -4041,11 +4035,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B13" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="24">
         <v>25</v>
       </c>
       <c r="D13" s="24">
@@ -4063,7 +4057,7 @@
       <c r="H13" s="24">
         <v>37</v>
       </c>
-      <c r="I13" s="54">
+      <c r="I13" s="24">
         <v>28</v>
       </c>
       <c r="J13" s="24">
@@ -4079,11 +4073,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B14" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="24">
         <v>32</v>
       </c>
       <c r="D14" s="24">
@@ -4101,7 +4095,7 @@
       <c r="H14" s="24">
         <v>60</v>
       </c>
-      <c r="I14" s="54">
+      <c r="I14" s="24">
         <v>36</v>
       </c>
       <c r="J14" s="24">
@@ -4117,11 +4111,11 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B15" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="24">
         <v>46</v>
       </c>
       <c r="D15" s="24">
@@ -4139,7 +4133,7 @@
       <c r="H15" s="24">
         <v>85</v>
       </c>
-      <c r="I15" s="54">
+      <c r="I15" s="24">
         <v>50</v>
       </c>
       <c r="J15" s="24">
@@ -4155,11 +4149,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B16" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="24">
         <v>40</v>
       </c>
       <c r="D16" s="24">
@@ -4177,7 +4171,7 @@
       <c r="H16" s="24">
         <v>34</v>
       </c>
-      <c r="I16" s="54">
+      <c r="I16" s="24">
         <v>44</v>
       </c>
       <c r="J16" s="24">
@@ -4193,11 +4187,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="24">
         <v>14</v>
       </c>
       <c r="D17" s="24">
@@ -4215,7 +4209,7 @@
       <c r="H17" s="24">
         <v>84</v>
       </c>
-      <c r="I17" s="54">
+      <c r="I17" s="24">
         <v>16</v>
       </c>
       <c r="J17" s="24">
@@ -4231,11 +4225,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B18" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="24">
         <v>21</v>
       </c>
       <c r="D18" s="24">
@@ -4253,7 +4247,7 @@
       <c r="H18" s="24">
         <v>47</v>
       </c>
-      <c r="I18" s="54">
+      <c r="I18" s="24">
         <v>24</v>
       </c>
       <c r="J18" s="24">
@@ -4269,11 +4263,11 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B19" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="24">
         <v>23</v>
       </c>
       <c r="D19" s="24">
@@ -4291,7 +4285,7 @@
       <c r="H19" s="24">
         <v>33</v>
       </c>
-      <c r="I19" s="54">
+      <c r="I19" s="24">
         <v>26</v>
       </c>
       <c r="J19" s="24">
@@ -4307,11 +4301,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B20" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="24">
         <v>43</v>
       </c>
       <c r="D20" s="24">
@@ -4329,7 +4323,7 @@
       <c r="H20" s="24">
         <v>42</v>
       </c>
-      <c r="I20" s="54">
+      <c r="I20" s="24">
         <v>47</v>
       </c>
       <c r="J20" s="24">
@@ -4345,11 +4339,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B21" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="24">
         <v>17</v>
       </c>
       <c r="D21" s="24">
@@ -4367,7 +4361,7 @@
       <c r="H21" s="24">
         <v>68</v>
       </c>
-      <c r="I21" s="54">
+      <c r="I21" s="24">
         <v>19</v>
       </c>
       <c r="J21" s="24">
@@ -4383,11 +4377,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B22" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="54">
+      <c r="C22" s="24">
         <v>22</v>
       </c>
       <c r="D22" s="24">
@@ -4405,7 +4399,7 @@
       <c r="H22" s="24">
         <v>49</v>
       </c>
-      <c r="I22" s="54">
+      <c r="I22" s="24">
         <v>25</v>
       </c>
       <c r="J22" s="24">
@@ -4421,11 +4415,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B23" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23" s="24">
         <v>27</v>
       </c>
       <c r="D23" s="24">
@@ -4443,7 +4437,7 @@
       <c r="H23" s="24">
         <v>24</v>
       </c>
-      <c r="I23" s="54">
+      <c r="I23" s="24">
         <v>31</v>
       </c>
       <c r="J23" s="24">
@@ -4459,11 +4453,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B24" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="24">
         <v>18</v>
       </c>
       <c r="D24" s="24">
@@ -4481,7 +4475,7 @@
       <c r="H24" s="24">
         <v>52</v>
       </c>
-      <c r="I24" s="54">
+      <c r="I24" s="24">
         <v>21</v>
       </c>
       <c r="J24" s="24">
@@ -4497,11 +4491,11 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B25" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="54">
+      <c r="C25" s="24">
         <v>33</v>
       </c>
       <c r="D25" s="24">
@@ -4519,7 +4513,7 @@
       <c r="H25" s="24">
         <v>37</v>
       </c>
-      <c r="I25" s="54">
+      <c r="I25" s="24">
         <v>37</v>
       </c>
       <c r="J25" s="24">
@@ -4535,11 +4529,11 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B26" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="54">
+      <c r="C26" s="24">
         <v>25</v>
       </c>
       <c r="D26" s="24">
@@ -4557,7 +4551,7 @@
       <c r="H26" s="24">
         <v>35</v>
       </c>
-      <c r="I26" s="54">
+      <c r="I26" s="24">
         <v>28</v>
       </c>
       <c r="J26" s="24">
@@ -4573,11 +4567,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B27" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="54">
+      <c r="C27" s="24">
         <v>50</v>
       </c>
       <c r="D27" s="24">
@@ -4595,7 +4589,7 @@
       <c r="H27" s="24">
         <v>55</v>
       </c>
-      <c r="I27" s="54">
+      <c r="I27" s="24">
         <v>56</v>
       </c>
       <c r="J27" s="24">
@@ -4611,11 +4605,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B28" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="54">
+      <c r="C28" s="24">
         <v>31</v>
       </c>
       <c r="D28" s="24">
@@ -4633,7 +4627,7 @@
       <c r="H28" s="24">
         <v>86</v>
       </c>
-      <c r="I28" s="54">
+      <c r="I28" s="24">
         <v>35</v>
       </c>
       <c r="J28" s="24">
@@ -4649,11 +4643,11 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B29" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="54">
+      <c r="C29" s="24">
         <v>21</v>
       </c>
       <c r="D29" s="24">
@@ -4671,7 +4665,7 @@
       <c r="H29" s="24">
         <v>54</v>
       </c>
-      <c r="I29" s="54">
+      <c r="I29" s="24">
         <v>24</v>
       </c>
       <c r="J29" s="24">
@@ -4687,11 +4681,11 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B30" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="54">
+      <c r="C30" s="24">
         <v>11</v>
       </c>
       <c r="D30" s="24">
@@ -4709,7 +4703,7 @@
       <c r="H30" s="24">
         <v>27</v>
       </c>
-      <c r="I30" s="54">
+      <c r="I30" s="24">
         <v>12</v>
       </c>
       <c r="J30" s="24">
@@ -4725,11 +4719,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B31" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="54">
+      <c r="C31" s="24">
         <v>54</v>
       </c>
       <c r="D31" s="24">
@@ -4747,7 +4741,7 @@
       <c r="H31" s="24">
         <v>32</v>
       </c>
-      <c r="I31" s="54">
+      <c r="I31" s="24">
         <v>60</v>
       </c>
       <c r="J31" s="24">
@@ -4763,15 +4757,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="B32" s="25"/>
-      <c r="C32" s="50"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
-      <c r="I32" s="50"/>
+      <c r="I32" s="19"/>
       <c r="J32" s="19"/>
       <c r="K32" s="19"/>
       <c r="L32" s="19"/>
@@ -4903,411 +4897,377 @@
       <selection sqref="A1:N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="49" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="18" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" style="49" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="48" customWidth="1"/>
-    <col min="10" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="49" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="4" width="16.453125" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="18" customWidth="1"/>
+    <col min="6" max="8" width="16.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="48" customWidth="1"/>
+    <col min="10" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="49"/>
-    </row>
-    <row r="2" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
-      <c r="B2" s="52" t="s">
+    <row r="1" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+    </row>
+    <row r="2" spans="1:15" ht="37" x14ac:dyDescent="0.35">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="52" t="s">
+      <c r="D2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="F2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="52" t="s">
+      <c r="G2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="52" t="s">
+      <c r="H2" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="52" t="s">
+      <c r="J2" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="L2" s="52" t="s">
+      <c r="L2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="52" t="s">
+      <c r="M2" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-    </row>
-    <row r="3" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="49"/>
-      <c r="B3" s="53" t="s">
+    </row>
+    <row r="3" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B3" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="24">
         <v>63</v>
       </c>
-      <c r="D3" s="54">
+      <c r="D3" s="24">
         <v>32</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="24">
         <v>75</v>
       </c>
-      <c r="F3" s="54">
+      <c r="F3" s="24">
         <v>86</v>
       </c>
-      <c r="G3" s="54">
+      <c r="G3" s="24">
         <v>41</v>
       </c>
-      <c r="H3" s="54">
+      <c r="H3" s="24">
         <v>28</v>
       </c>
-      <c r="I3" s="58">
+      <c r="I3" s="51">
         <v>36</v>
       </c>
-      <c r="J3" s="54">
+      <c r="J3" s="24">
         <v>57</v>
       </c>
-      <c r="K3" s="54">
+      <c r="K3" s="24">
         <v>70</v>
       </c>
-      <c r="L3" s="54">
+      <c r="L3" s="24">
         <v>23</v>
       </c>
-      <c r="M3" s="54">
+      <c r="M3" s="24">
         <v>88</v>
       </c>
-      <c r="N3" s="49"/>
-      <c r="O3" s="49"/>
-    </row>
-    <row r="4" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
-      <c r="B4" s="53" t="s">
+    </row>
+    <row r="4" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B4" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="24">
         <v>36</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="24">
         <v>31</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="24">
         <v>65</v>
       </c>
-      <c r="F4" s="54">
+      <c r="F4" s="24">
         <v>59</v>
       </c>
-      <c r="G4" s="54">
+      <c r="G4" s="24">
         <v>40</v>
       </c>
-      <c r="H4" s="54">
+      <c r="H4" s="24">
         <v>51</v>
       </c>
-      <c r="I4" s="58">
+      <c r="I4" s="51">
         <v>15</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J4" s="24">
         <v>19</v>
       </c>
-      <c r="K4" s="54">
+      <c r="K4" s="24">
         <v>40</v>
       </c>
-      <c r="L4" s="54">
+      <c r="L4" s="24">
         <v>36</v>
       </c>
-      <c r="M4" s="54">
+      <c r="M4" s="24">
         <v>44</v>
       </c>
-      <c r="N4" s="49"/>
-      <c r="O4" s="49"/>
-    </row>
-    <row r="5" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="53" t="s">
+    </row>
+    <row r="5" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B5" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="24">
         <v>18</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="24">
         <v>25</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="24">
         <v>62</v>
       </c>
-      <c r="F5" s="54">
+      <c r="F5" s="24">
         <v>61</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="24">
         <v>37</v>
       </c>
-      <c r="H5" s="54">
+      <c r="H5" s="24">
         <v>62</v>
       </c>
-      <c r="I5" s="58">
+      <c r="I5" s="51">
         <v>25</v>
       </c>
-      <c r="J5" s="54">
+      <c r="J5" s="24">
         <v>45</v>
       </c>
-      <c r="K5" s="54">
+      <c r="K5" s="24">
         <v>32</v>
       </c>
-      <c r="L5" s="54">
+      <c r="L5" s="24">
         <v>24</v>
       </c>
-      <c r="M5" s="54">
+      <c r="M5" s="24">
         <v>16</v>
       </c>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-    </row>
-    <row r="6" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
-      <c r="B6" s="53" t="s">
+    </row>
+    <row r="6" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="24">
         <v>21</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="24">
         <v>23</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="24">
         <v>97</v>
       </c>
-      <c r="F6" s="54">
+      <c r="F6" s="24">
         <v>33</v>
       </c>
-      <c r="G6" s="54">
+      <c r="G6" s="24">
         <v>33</v>
       </c>
-      <c r="H6" s="54">
+      <c r="H6" s="24">
         <v>70</v>
       </c>
-      <c r="I6" s="58">
+      <c r="I6" s="51">
         <v>29</v>
       </c>
-      <c r="J6" s="54">
+      <c r="J6" s="24">
         <v>40</v>
       </c>
-      <c r="K6" s="54">
+      <c r="K6" s="24">
         <v>24</v>
       </c>
-      <c r="L6" s="54">
+      <c r="L6" s="24">
         <v>11</v>
       </c>
-      <c r="M6" s="54">
+      <c r="M6" s="24">
         <v>24</v>
       </c>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-    </row>
-    <row r="7" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="53" t="s">
+    </row>
+    <row r="7" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="24">
         <v>22</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="24">
         <v>19</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="24">
         <v>36</v>
       </c>
-      <c r="F7" s="54">
+      <c r="F7" s="24">
         <v>43</v>
       </c>
-      <c r="G7" s="54">
+      <c r="G7" s="24">
         <v>87</v>
       </c>
-      <c r="H7" s="54">
+      <c r="H7" s="24">
         <v>29</v>
       </c>
-      <c r="I7" s="58">
+      <c r="I7" s="51">
         <v>22</v>
       </c>
-      <c r="J7" s="54">
+      <c r="J7" s="24">
         <v>20</v>
       </c>
-      <c r="K7" s="54">
+      <c r="K7" s="24">
         <v>25</v>
       </c>
-      <c r="L7" s="54">
+      <c r="L7" s="24">
         <v>23</v>
       </c>
-      <c r="M7" s="54">
+      <c r="M7" s="24">
         <v>47</v>
       </c>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-    </row>
-    <row r="8" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="53" t="s">
+    </row>
+    <row r="8" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B8" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="24">
         <v>61</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="24">
         <v>25</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="24">
         <v>53</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="24">
         <v>55</v>
       </c>
-      <c r="G8" s="54">
+      <c r="G8" s="24">
         <v>90</v>
       </c>
-      <c r="H8" s="54">
+      <c r="H8" s="24">
         <v>65</v>
       </c>
-      <c r="I8" s="58">
+      <c r="I8" s="51">
         <v>50</v>
       </c>
-      <c r="J8" s="54">
+      <c r="J8" s="24">
         <v>65</v>
       </c>
-      <c r="K8" s="54">
+      <c r="K8" s="24">
         <v>68</v>
       </c>
-      <c r="L8" s="54">
+      <c r="L8" s="24">
         <v>41</v>
       </c>
-      <c r="M8" s="54">
+      <c r="M8" s="24">
         <v>63</v>
       </c>
-      <c r="N8" s="49"/>
-      <c r="O8" s="49"/>
-    </row>
-    <row r="9" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="53" t="s">
+    </row>
+    <row r="9" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B9" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="24">
         <v>20</v>
       </c>
-      <c r="D9" s="54">
+      <c r="D9" s="24">
         <v>46</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="24">
         <v>58</v>
       </c>
-      <c r="F9" s="54">
+      <c r="F9" s="24">
         <v>69</v>
       </c>
-      <c r="G9" s="54">
+      <c r="G9" s="24">
         <v>85</v>
       </c>
-      <c r="H9" s="54">
+      <c r="H9" s="24">
         <v>18</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="51">
         <v>27</v>
       </c>
-      <c r="J9" s="54">
+      <c r="J9" s="24">
         <v>27</v>
       </c>
-      <c r="K9" s="54">
+      <c r="K9" s="24">
         <v>23</v>
       </c>
-      <c r="L9" s="54">
+      <c r="L9" s="24">
         <v>38</v>
       </c>
-      <c r="M9" s="54">
+      <c r="M9" s="24">
         <v>40</v>
       </c>
-      <c r="N9" s="49"/>
-      <c r="O9" s="49"/>
-    </row>
-    <row r="10" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="53" t="s">
+    </row>
+    <row r="10" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B10" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="24">
         <v>58</v>
       </c>
-      <c r="D10" s="54">
+      <c r="D10" s="24">
         <v>33</v>
       </c>
-      <c r="E10" s="54">
+      <c r="E10" s="24">
         <v>95</v>
       </c>
-      <c r="F10" s="54">
+      <c r="F10" s="24">
         <v>34</v>
       </c>
-      <c r="G10" s="54">
+      <c r="G10" s="24">
         <v>37</v>
       </c>
-      <c r="H10" s="54">
+      <c r="H10" s="24">
         <v>59</v>
       </c>
-      <c r="I10" s="58">
+      <c r="I10" s="51">
         <v>37</v>
       </c>
-      <c r="J10" s="54">
+      <c r="J10" s="24">
         <v>39</v>
       </c>
-      <c r="K10" s="54">
+      <c r="K10" s="24">
         <v>65</v>
       </c>
-      <c r="L10" s="54">
+      <c r="L10" s="24">
         <v>42</v>
       </c>
-      <c r="M10" s="54">
+      <c r="M10" s="24">
         <v>67</v>
       </c>
-      <c r="N10" s="49"/>
-      <c r="O10" s="49"/>
-    </row>
-    <row r="11" spans="1:15" s="47" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="59" t="s">
+    </row>
+    <row r="11" spans="1:15" s="47" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B11" s="52" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="46">
@@ -5344,843 +5304,791 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="53" t="s">
+    <row r="12" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="24">
         <v>38</v>
       </c>
-      <c r="D12" s="54">
+      <c r="D12" s="24">
         <v>32</v>
       </c>
-      <c r="E12" s="54">
+      <c r="E12" s="24">
         <v>48</v>
       </c>
-      <c r="F12" s="54">
+      <c r="F12" s="24">
         <v>65</v>
       </c>
-      <c r="G12" s="54">
+      <c r="G12" s="24">
         <v>60</v>
       </c>
-      <c r="H12" s="54">
+      <c r="H12" s="24">
         <v>45</v>
       </c>
-      <c r="I12" s="58">
+      <c r="I12" s="51">
         <v>36</v>
       </c>
-      <c r="J12" s="54">
+      <c r="J12" s="24">
         <v>15</v>
       </c>
-      <c r="K12" s="54">
+      <c r="K12" s="24">
         <v>43</v>
       </c>
-      <c r="L12" s="54">
+      <c r="L12" s="24">
         <v>37</v>
       </c>
-      <c r="M12" s="54">
+      <c r="M12" s="24">
         <v>55</v>
       </c>
-      <c r="N12" s="49"/>
-      <c r="O12" s="49"/>
-    </row>
-    <row r="13" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="53" t="s">
+    </row>
+    <row r="13" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B13" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="24">
         <v>24</v>
       </c>
-      <c r="D13" s="54">
+      <c r="D13" s="24">
         <v>40</v>
       </c>
-      <c r="E13" s="54">
+      <c r="E13" s="24">
         <v>50</v>
       </c>
-      <c r="F13" s="54">
+      <c r="F13" s="24">
         <v>40</v>
       </c>
-      <c r="G13" s="54">
+      <c r="G13" s="24">
         <v>34</v>
       </c>
-      <c r="H13" s="54">
+      <c r="H13" s="24">
         <v>29</v>
       </c>
-      <c r="I13" s="58">
+      <c r="I13" s="51">
         <v>44</v>
       </c>
-      <c r="J13" s="54">
+      <c r="J13" s="24">
         <v>73</v>
       </c>
-      <c r="K13" s="54">
+      <c r="K13" s="24">
         <v>27</v>
       </c>
-      <c r="L13" s="54">
+      <c r="L13" s="24">
         <v>28</v>
       </c>
-      <c r="M13" s="54">
+      <c r="M13" s="24">
         <v>70</v>
       </c>
-      <c r="N13" s="49"/>
-      <c r="O13" s="49"/>
-    </row>
-    <row r="14" spans="1:15" s="49" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="53" t="s">
+    </row>
+    <row r="14" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B14" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="54">
+      <c r="C14" s="24">
         <v>52</v>
       </c>
-      <c r="D14" s="54">
+      <c r="D14" s="24">
         <v>27</v>
       </c>
-      <c r="E14" s="54">
+      <c r="E14" s="24">
         <v>49</v>
       </c>
-      <c r="F14" s="54">
+      <c r="F14" s="24">
         <v>46</v>
       </c>
-      <c r="G14" s="54">
+      <c r="G14" s="24">
         <v>24</v>
       </c>
-      <c r="H14" s="54">
+      <c r="H14" s="24">
         <v>73</v>
       </c>
-      <c r="I14" s="58">
+      <c r="I14" s="51">
         <v>31</v>
       </c>
-      <c r="J14" s="54">
+      <c r="J14" s="24">
         <v>18</v>
       </c>
-      <c r="K14" s="54">
+      <c r="K14" s="24">
         <v>59</v>
       </c>
-      <c r="L14" s="54">
+      <c r="L14" s="24">
         <v>74</v>
       </c>
-      <c r="M14" s="54">
+      <c r="M14" s="24">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="47" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="53" t="s">
+    <row r="15" spans="1:15" s="47" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A15"/>
+      <c r="B15" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="24">
         <v>64</v>
       </c>
-      <c r="D15" s="54">
+      <c r="D15" s="24">
         <v>50</v>
       </c>
-      <c r="E15" s="54">
+      <c r="E15" s="24">
         <v>50</v>
       </c>
-      <c r="F15" s="54">
+      <c r="F15" s="24">
         <v>42</v>
       </c>
-      <c r="G15" s="54">
+      <c r="G15" s="24">
         <v>55</v>
       </c>
-      <c r="H15" s="54">
+      <c r="H15" s="24">
         <v>71</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="51">
         <v>56</v>
       </c>
-      <c r="J15" s="54">
+      <c r="J15" s="24">
         <v>34</v>
       </c>
-      <c r="K15" s="54">
+      <c r="K15" s="24">
         <v>71</v>
       </c>
-      <c r="L15" s="54">
+      <c r="L15" s="24">
         <v>63</v>
       </c>
-      <c r="M15" s="54">
+      <c r="M15" s="24">
         <v>63</v>
       </c>
-      <c r="N15" s="49"/>
-      <c r="O15" s="49"/>
-    </row>
-    <row r="16" spans="1:15" s="45" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="53" t="s">
+      <c r="N15"/>
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:15" s="45" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A16"/>
+      <c r="B16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="24">
         <v>46</v>
       </c>
-      <c r="D16" s="54">
+      <c r="D16" s="24">
         <v>36</v>
       </c>
-      <c r="E16" s="54">
+      <c r="E16" s="24">
         <v>63</v>
       </c>
-      <c r="F16" s="54">
+      <c r="F16" s="24">
         <v>77</v>
       </c>
-      <c r="G16" s="54">
+      <c r="G16" s="24">
         <v>46</v>
       </c>
-      <c r="H16" s="54">
+      <c r="H16" s="24">
         <v>49</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="51">
         <v>40</v>
       </c>
-      <c r="J16" s="54">
+      <c r="J16" s="24">
         <v>57</v>
       </c>
-      <c r="K16" s="54">
+      <c r="K16" s="24">
         <v>53</v>
       </c>
-      <c r="L16" s="54">
+      <c r="L16" s="24">
         <v>14</v>
       </c>
-      <c r="M16" s="54">
+      <c r="M16" s="24">
         <v>64</v>
       </c>
-      <c r="N16" s="49"/>
-      <c r="O16" s="49"/>
-    </row>
-    <row r="17" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="53" t="s">
+      <c r="N16"/>
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="24">
         <v>18</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="24">
         <v>18</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="24">
         <v>90</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="24">
         <v>73</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="24">
         <v>52</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="24">
         <v>68</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="51">
         <v>21</v>
       </c>
-      <c r="J17" s="54">
+      <c r="J17" s="24">
         <v>42</v>
       </c>
-      <c r="K17" s="54">
+      <c r="K17" s="24">
         <v>21</v>
       </c>
-      <c r="L17" s="54">
+      <c r="L17" s="24">
         <v>27</v>
       </c>
-      <c r="M17" s="54">
+      <c r="M17" s="24">
         <v>33</v>
       </c>
-      <c r="N17" s="49"/>
-      <c r="O17" s="49"/>
-    </row>
-    <row r="18" spans="1:15" s="47" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="53" t="s">
+    </row>
+    <row r="18" spans="1:15" s="47" customFormat="1" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="A18"/>
+      <c r="B18" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="24">
         <v>37</v>
       </c>
-      <c r="D18" s="54">
+      <c r="D18" s="24">
         <v>47</v>
       </c>
-      <c r="E18" s="54">
+      <c r="E18" s="24">
         <v>39</v>
       </c>
-      <c r="F18" s="54">
+      <c r="F18" s="24">
         <v>27</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="24">
         <v>25</v>
       </c>
-      <c r="H18" s="54">
+      <c r="H18" s="24">
         <v>75</v>
       </c>
-      <c r="I18" s="58">
+      <c r="I18" s="51">
         <v>53</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J18" s="24">
         <v>39</v>
       </c>
-      <c r="K18" s="54">
+      <c r="K18" s="24">
         <v>42</v>
       </c>
-      <c r="L18" s="54">
+      <c r="L18" s="24">
         <v>65</v>
       </c>
-      <c r="M18" s="54">
+      <c r="M18" s="24">
         <v>64</v>
       </c>
-      <c r="N18" s="49"/>
-      <c r="O18" s="49"/>
-    </row>
-    <row r="19" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="53" t="s">
+      <c r="N18"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B19" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="24">
         <v>18</v>
       </c>
-      <c r="D19" s="54">
+      <c r="D19" s="24">
         <v>17</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="24">
         <v>86</v>
       </c>
-      <c r="F19" s="54">
+      <c r="F19" s="24">
         <v>50</v>
       </c>
-      <c r="G19" s="54">
+      <c r="G19" s="24">
         <v>38</v>
       </c>
-      <c r="H19" s="54">
+      <c r="H19" s="24">
         <v>50</v>
       </c>
-      <c r="I19" s="58">
+      <c r="I19" s="51">
         <v>19</v>
       </c>
-      <c r="J19" s="54">
+      <c r="J19" s="24">
         <v>52</v>
       </c>
-      <c r="K19" s="54">
+      <c r="K19" s="24">
         <v>21</v>
       </c>
-      <c r="L19" s="54">
+      <c r="L19" s="24">
         <v>25</v>
       </c>
-      <c r="M19" s="54">
+      <c r="M19" s="24">
         <v>65</v>
       </c>
-      <c r="N19" s="49"/>
-      <c r="O19" s="49"/>
-    </row>
-    <row r="20" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="53" t="s">
+    </row>
+    <row r="20" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="24">
         <v>32</v>
       </c>
-      <c r="D20" s="54">
+      <c r="D20" s="24">
         <v>43</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="24">
         <v>67</v>
       </c>
-      <c r="F20" s="54">
+      <c r="F20" s="24">
         <v>37</v>
       </c>
-      <c r="G20" s="54">
+      <c r="G20" s="24">
         <v>42</v>
       </c>
-      <c r="H20" s="54">
+      <c r="H20" s="24">
         <v>27</v>
       </c>
-      <c r="I20" s="58">
+      <c r="I20" s="51">
         <v>47</v>
       </c>
-      <c r="J20" s="54">
+      <c r="J20" s="24">
         <v>37</v>
       </c>
-      <c r="K20" s="54">
+      <c r="K20" s="24">
         <v>36</v>
       </c>
-      <c r="L20" s="54">
+      <c r="L20" s="24">
         <v>25</v>
       </c>
-      <c r="M20" s="54">
+      <c r="M20" s="24">
         <v>45</v>
       </c>
-      <c r="N20" s="49"/>
-      <c r="O20" s="49"/>
-    </row>
-    <row r="21" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
-      <c r="B21" s="53" t="s">
+    </row>
+    <row r="21" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="24">
         <v>37</v>
       </c>
-      <c r="D21" s="54">
+      <c r="D21" s="24">
         <v>17</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="24">
         <v>36</v>
       </c>
-      <c r="F21" s="54">
+      <c r="F21" s="24">
         <v>47</v>
       </c>
-      <c r="G21" s="54">
+      <c r="G21" s="24">
         <v>41</v>
       </c>
-      <c r="H21" s="54">
+      <c r="H21" s="24">
         <v>37</v>
       </c>
-      <c r="I21" s="58">
+      <c r="I21" s="51">
         <v>19</v>
       </c>
-      <c r="J21" s="54">
+      <c r="J21" s="24">
         <v>59</v>
       </c>
-      <c r="K21" s="54">
+      <c r="K21" s="24">
         <v>42</v>
       </c>
-      <c r="L21" s="54">
+      <c r="L21" s="24">
         <v>14</v>
       </c>
-      <c r="M21" s="54">
+      <c r="M21" s="24">
         <v>33</v>
       </c>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-    </row>
-    <row r="22" spans="1:15" s="49" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B22" s="53" t="s">
+    </row>
+    <row r="22" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="54">
+      <c r="C22" s="24">
         <v>36</v>
       </c>
-      <c r="D22" s="54">
+      <c r="D22" s="24">
         <v>22</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="24">
         <v>41</v>
       </c>
-      <c r="F22" s="54">
+      <c r="F22" s="24">
         <v>29</v>
       </c>
-      <c r="G22" s="54">
+      <c r="G22" s="24">
         <v>49</v>
       </c>
-      <c r="H22" s="54">
+      <c r="H22" s="24">
         <v>52</v>
       </c>
-      <c r="I22" s="58">
+      <c r="I22" s="51">
         <v>25</v>
       </c>
-      <c r="J22" s="54">
+      <c r="J22" s="24">
         <v>50</v>
       </c>
-      <c r="K22" s="54">
+      <c r="K22" s="24">
         <v>41</v>
       </c>
-      <c r="L22" s="54">
+      <c r="L22" s="24">
         <v>45</v>
       </c>
-      <c r="M22" s="54">
+      <c r="M22" s="24">
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="49" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B23" s="53" t="s">
+    <row r="23" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="54">
+      <c r="C23" s="24">
         <v>42</v>
       </c>
-      <c r="D23" s="54">
+      <c r="D23" s="24">
         <v>54</v>
       </c>
-      <c r="E23" s="54">
+      <c r="E23" s="24">
         <v>79</v>
       </c>
-      <c r="F23" s="54">
+      <c r="F23" s="24">
         <v>88</v>
       </c>
-      <c r="G23" s="54">
+      <c r="G23" s="24">
         <v>32</v>
       </c>
-      <c r="H23" s="54">
+      <c r="H23" s="24">
         <v>16</v>
       </c>
-      <c r="I23" s="58">
+      <c r="I23" s="51">
         <v>60</v>
       </c>
-      <c r="J23" s="54">
+      <c r="J23" s="24">
         <v>72</v>
       </c>
-      <c r="K23" s="54">
+      <c r="K23" s="24">
         <v>47</v>
       </c>
-      <c r="L23" s="54">
+      <c r="L23" s="24">
         <v>73</v>
       </c>
-      <c r="M23" s="54">
+      <c r="M23" s="24">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="49"/>
-      <c r="B24" s="53" t="s">
+    <row r="24" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="54">
+      <c r="C24" s="24">
         <v>42</v>
       </c>
-      <c r="D24" s="54">
+      <c r="D24" s="24">
         <v>21</v>
       </c>
-      <c r="E24" s="54">
+      <c r="E24" s="24">
         <v>49</v>
       </c>
-      <c r="F24" s="54">
+      <c r="F24" s="24">
         <v>80</v>
       </c>
-      <c r="G24" s="54">
+      <c r="G24" s="24">
         <v>54</v>
       </c>
-      <c r="H24" s="54">
+      <c r="H24" s="24">
         <v>17</v>
       </c>
-      <c r="I24" s="58">
+      <c r="I24" s="51">
         <v>24</v>
       </c>
-      <c r="J24" s="54">
+      <c r="J24" s="24">
         <v>69</v>
       </c>
-      <c r="K24" s="54">
+      <c r="K24" s="24">
         <v>47</v>
       </c>
-      <c r="L24" s="54">
+      <c r="L24" s="24">
         <v>33</v>
       </c>
-      <c r="M24" s="54">
+      <c r="M24" s="24">
         <v>64</v>
       </c>
-      <c r="N24" s="49"/>
-      <c r="O24" s="49"/>
-    </row>
-    <row r="25" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="49"/>
-      <c r="B25" s="53" t="s">
+    </row>
+    <row r="25" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="54">
+      <c r="C25" s="24">
         <v>14</v>
       </c>
-      <c r="D25" s="54">
+      <c r="D25" s="24">
         <v>46</v>
       </c>
-      <c r="E25" s="54">
+      <c r="E25" s="24">
         <v>83</v>
       </c>
-      <c r="F25" s="54">
+      <c r="F25" s="24">
         <v>45</v>
       </c>
-      <c r="G25" s="54">
+      <c r="G25" s="24">
         <v>30</v>
       </c>
-      <c r="H25" s="54">
+      <c r="H25" s="24">
         <v>28</v>
       </c>
-      <c r="I25" s="58">
+      <c r="I25" s="51">
         <v>51</v>
       </c>
-      <c r="J25" s="54">
+      <c r="J25" s="24">
         <v>35</v>
       </c>
-      <c r="K25" s="54">
+      <c r="K25" s="24">
         <v>16</v>
       </c>
-      <c r="L25" s="54">
+      <c r="L25" s="24">
         <v>40</v>
       </c>
-      <c r="M25" s="54">
+      <c r="M25" s="24">
         <v>82</v>
       </c>
-      <c r="N25" s="49"/>
-      <c r="O25" s="49"/>
-    </row>
-    <row r="26" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="49"/>
-      <c r="B26" s="53" t="s">
+    </row>
+    <row r="26" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="54">
+      <c r="C26" s="24">
         <v>25</v>
       </c>
-      <c r="D26" s="54">
+      <c r="D26" s="24">
         <v>11</v>
       </c>
-      <c r="E26" s="54">
+      <c r="E26" s="24">
         <v>66</v>
       </c>
-      <c r="F26" s="54">
+      <c r="F26" s="24">
         <v>61</v>
       </c>
-      <c r="G26" s="54">
+      <c r="G26" s="24">
         <v>27</v>
       </c>
-      <c r="H26" s="54">
+      <c r="H26" s="24">
         <v>25</v>
       </c>
-      <c r="I26" s="58">
+      <c r="I26" s="51">
         <v>12</v>
       </c>
-      <c r="J26" s="54">
+      <c r="J26" s="24">
         <v>20</v>
       </c>
-      <c r="K26" s="54">
+      <c r="K26" s="24">
         <v>28</v>
       </c>
-      <c r="L26" s="54">
+      <c r="L26" s="24">
         <v>15</v>
       </c>
-      <c r="M26" s="54">
+      <c r="M26" s="24">
         <v>34</v>
       </c>
-      <c r="N26" s="49"/>
-      <c r="O26" s="49"/>
-    </row>
-    <row r="27" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="49"/>
-      <c r="B27" s="53" t="s">
+    </row>
+    <row r="27" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="54">
+      <c r="C27" s="24">
         <v>55</v>
       </c>
-      <c r="D27" s="54">
+      <c r="D27" s="24">
         <v>17</v>
       </c>
-      <c r="E27" s="54">
+      <c r="E27" s="24">
         <v>68</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F27" s="24">
         <v>20</v>
       </c>
-      <c r="G27" s="54">
+      <c r="G27" s="24">
         <v>68</v>
       </c>
-      <c r="H27" s="54">
+      <c r="H27" s="24">
         <v>35</v>
       </c>
-      <c r="I27" s="58">
+      <c r="I27" s="51">
         <v>19</v>
       </c>
-      <c r="J27" s="54">
+      <c r="J27" s="24">
         <v>54</v>
       </c>
-      <c r="K27" s="54">
+      <c r="K27" s="24">
         <v>62</v>
       </c>
-      <c r="L27" s="54">
+      <c r="L27" s="24">
         <v>59</v>
       </c>
-      <c r="M27" s="54">
+      <c r="M27" s="24">
         <v>63</v>
       </c>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
-    </row>
-    <row r="28" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="49"/>
-      <c r="B28" s="53" t="s">
+    </row>
+    <row r="28" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B28" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="54">
+      <c r="C28" s="24">
         <v>13</v>
       </c>
-      <c r="D28" s="54">
+      <c r="D28" s="24">
         <v>21</v>
       </c>
-      <c r="E28" s="54">
+      <c r="E28" s="24">
         <v>98</v>
       </c>
-      <c r="F28" s="54">
+      <c r="F28" s="24">
         <v>46</v>
       </c>
-      <c r="G28" s="54">
+      <c r="G28" s="24">
         <v>47</v>
       </c>
-      <c r="H28" s="54">
+      <c r="H28" s="24">
         <v>26</v>
       </c>
-      <c r="I28" s="58">
+      <c r="I28" s="51">
         <v>24</v>
       </c>
-      <c r="J28" s="54">
+      <c r="J28" s="24">
         <v>32</v>
       </c>
-      <c r="K28" s="54">
+      <c r="K28" s="24">
         <v>15</v>
       </c>
-      <c r="L28" s="54">
+      <c r="L28" s="24">
         <v>41</v>
       </c>
-      <c r="M28" s="54">
+      <c r="M28" s="24">
         <v>32</v>
       </c>
-      <c r="N28" s="49"/>
-      <c r="O28" s="49"/>
-    </row>
-    <row r="29" spans="1:15" s="49" customFormat="1" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="B29" s="53" t="s">
+    </row>
+    <row r="29" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="54">
+      <c r="C29" s="24">
         <v>33</v>
       </c>
-      <c r="D29" s="54">
+      <c r="D29" s="24">
         <v>25</v>
       </c>
-      <c r="E29" s="54">
+      <c r="E29" s="24">
         <v>43</v>
       </c>
-      <c r="F29" s="54">
+      <c r="F29" s="24">
         <v>50</v>
       </c>
-      <c r="G29" s="54">
+      <c r="G29" s="24">
         <v>35</v>
       </c>
-      <c r="H29" s="54">
+      <c r="H29" s="24">
         <v>50</v>
       </c>
-      <c r="I29" s="58">
+      <c r="I29" s="51">
         <v>28</v>
       </c>
-      <c r="J29" s="54">
+      <c r="J29" s="24">
         <v>42</v>
       </c>
-      <c r="K29" s="54">
+      <c r="K29" s="24">
         <v>37</v>
       </c>
-      <c r="L29" s="54">
+      <c r="L29" s="24">
         <v>70</v>
       </c>
-      <c r="M29" s="54">
+      <c r="M29" s="24">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="49"/>
-      <c r="B30" s="53" t="s">
+    <row r="30" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B30" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="54">
+      <c r="C30" s="24">
         <v>21</v>
       </c>
-      <c r="D30" s="54">
+      <c r="D30" s="24">
         <v>14</v>
       </c>
-      <c r="E30" s="54">
+      <c r="E30" s="24">
         <v>40</v>
       </c>
-      <c r="F30" s="54">
+      <c r="F30" s="24">
         <v>22</v>
       </c>
-      <c r="G30" s="54">
+      <c r="G30" s="24">
         <v>84</v>
       </c>
-      <c r="H30" s="54">
+      <c r="H30" s="24">
         <v>20</v>
       </c>
-      <c r="I30" s="58">
+      <c r="I30" s="51">
         <v>16</v>
       </c>
-      <c r="J30" s="54">
+      <c r="J30" s="24">
         <v>98</v>
       </c>
-      <c r="K30" s="54">
+      <c r="K30" s="24">
         <v>24</v>
       </c>
-      <c r="L30" s="54">
+      <c r="L30" s="24">
         <v>56</v>
       </c>
-      <c r="M30" s="54">
+      <c r="M30" s="24">
         <v>63</v>
       </c>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-    </row>
-    <row r="31" spans="1:15" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="49"/>
-      <c r="B31" s="53" t="s">
+    </row>
+    <row r="31" spans="1:15" ht="19.5" x14ac:dyDescent="0.45">
+      <c r="B31" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="54">
+      <c r="C31" s="24">
         <v>38</v>
       </c>
-      <c r="D31" s="54">
+      <c r="D31" s="24">
         <v>15</v>
       </c>
-      <c r="E31" s="54">
+      <c r="E31" s="24">
         <v>91</v>
       </c>
-      <c r="F31" s="54">
+      <c r="F31" s="24">
         <v>83</v>
       </c>
-      <c r="G31" s="54">
+      <c r="G31" s="24">
         <v>78</v>
       </c>
-      <c r="H31" s="54">
+      <c r="H31" s="24">
         <v>31</v>
       </c>
-      <c r="I31" s="58">
+      <c r="I31" s="51">
         <v>17</v>
       </c>
-      <c r="J31" s="54">
+      <c r="J31" s="24">
         <v>62</v>
       </c>
-      <c r="K31" s="54">
+      <c r="K31" s="24">
         <v>43</v>
       </c>
-      <c r="L31" s="54">
+      <c r="L31" s="24">
         <v>38</v>
       </c>
-      <c r="M31" s="54">
+      <c r="M31" s="24">
         <v>35</v>
       </c>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-    </row>
-    <row r="32" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="49"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="50"/>
-      <c r="I32" s="56"/>
-      <c r="J32" s="50"/>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
-      <c r="M32" s="50"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="49"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="49"/>
-      <c r="B33" s="49"/>
-      <c r="C33" s="49"/>
-      <c r="E33" s="49"/>
-      <c r="F33" s="49"/>
-      <c r="H33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
+    </row>
+    <row r="32" spans="1:15" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="B32" s="25"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="E33"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
@@ -6305,15 +6213,15 @@
       <selection sqref="A1:N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -6327,7 +6235,7 @@
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="37" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="22" t="s">
         <v>28</v>
@@ -6366,7 +6274,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B3" s="26" t="s">
         <v>67</v>
       </c>
@@ -6404,7 +6312,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B4" s="23" t="s">
         <v>53</v>
       </c>
@@ -6442,7 +6350,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B5" s="26" t="s">
         <v>66</v>
       </c>
@@ -6480,7 +6388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B6" s="23" t="s">
         <v>63</v>
       </c>
@@ -6518,7 +6426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B7" s="26" t="s">
         <v>45</v>
       </c>
@@ -6556,7 +6464,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B8" s="23" t="s">
         <v>60</v>
       </c>
@@ -6594,7 +6502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B9" s="26" t="s">
         <v>50</v>
       </c>
@@ -6632,7 +6540,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B10" s="23" t="s">
         <v>48</v>
       </c>
@@ -6670,7 +6578,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B11" s="26" t="s">
         <v>57</v>
       </c>
@@ -6708,7 +6616,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B12" s="23" t="s">
         <v>65</v>
       </c>
@@ -6746,7 +6654,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B13" s="26" t="s">
         <v>43</v>
       </c>
@@ -6784,7 +6692,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B14" s="23" t="s">
         <v>62</v>
       </c>
@@ -6822,7 +6730,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B15" s="26" t="s">
         <v>61</v>
       </c>
@@ -6860,7 +6768,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B16" s="23" t="s">
         <v>64</v>
       </c>
@@ -6898,7 +6806,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B17" s="26" t="s">
         <v>40</v>
       </c>
@@ -6936,7 +6844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B18" s="23" t="s">
         <v>55</v>
       </c>
@@ -6974,7 +6882,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B19" s="26" t="s">
         <v>41</v>
       </c>
@@ -7012,7 +6920,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B20" s="23" t="s">
         <v>56</v>
       </c>
@@ -7050,7 +6958,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B21" s="26" t="s">
         <v>42</v>
       </c>
@@ -7088,7 +6996,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B22" s="23" t="s">
         <v>52</v>
       </c>
@@ -7126,7 +7034,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B23" s="26" t="s">
         <v>51</v>
       </c>
@@ -7164,7 +7072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B24" s="23" t="s">
         <v>47</v>
       </c>
@@ -7202,7 +7110,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B25" s="26" t="s">
         <v>58</v>
       </c>
@@ -7240,7 +7148,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B26" s="23" t="s">
         <v>44</v>
       </c>
@@ -7278,7 +7186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B27" s="26" t="s">
         <v>68</v>
       </c>
@@ -7316,7 +7224,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B28" s="23" t="s">
         <v>46</v>
       </c>
@@ -7354,7 +7262,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B29" s="26" t="s">
         <v>49</v>
       </c>
@@ -7392,7 +7300,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B30" s="23" t="s">
         <v>54</v>
       </c>
@@ -7430,7 +7338,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B31" s="26" t="s">
         <v>59</v>
       </c>
@@ -7468,7 +7376,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="B32" s="25"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -7605,15 +7513,15 @@
       <selection sqref="A1:N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -7627,7 +7535,7 @@
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="37" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="21" t="s">
         <v>28</v>
@@ -7666,7 +7574,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B3" s="23" t="s">
         <v>67</v>
       </c>
@@ -7704,7 +7612,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B4" s="23" t="s">
         <v>53</v>
       </c>
@@ -7742,7 +7650,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B5" s="23" t="s">
         <v>66</v>
       </c>
@@ -7780,7 +7688,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B6" s="23" t="s">
         <v>63</v>
       </c>
@@ -7818,7 +7726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B7" s="23" t="s">
         <v>45</v>
       </c>
@@ -7856,7 +7764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B8" s="23" t="s">
         <v>60</v>
       </c>
@@ -7894,7 +7802,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B9" s="23" t="s">
         <v>50</v>
       </c>
@@ -7932,7 +7840,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B10" s="23" t="s">
         <v>48</v>
       </c>
@@ -7970,7 +7878,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B11" s="23" t="s">
         <v>57</v>
       </c>
@@ -8008,7 +7916,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B12" s="23" t="s">
         <v>65</v>
       </c>
@@ -8046,7 +7954,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B13" s="23" t="s">
         <v>43</v>
       </c>
@@ -8084,7 +7992,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B14" s="23" t="s">
         <v>62</v>
       </c>
@@ -8122,7 +8030,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B15" s="23" t="s">
         <v>61</v>
       </c>
@@ -8160,7 +8068,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B16" s="23" t="s">
         <v>64</v>
       </c>
@@ -8198,7 +8106,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B17" s="23" t="s">
         <v>40</v>
       </c>
@@ -8236,7 +8144,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B18" s="23" t="s">
         <v>55</v>
       </c>
@@ -8274,7 +8182,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B19" s="23" t="s">
         <v>41</v>
       </c>
@@ -8312,7 +8220,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B20" s="23" t="s">
         <v>56</v>
       </c>
@@ -8350,7 +8258,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B21" s="23" t="s">
         <v>42</v>
       </c>
@@ -8388,7 +8296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B22" s="23" t="s">
         <v>52</v>
       </c>
@@ -8426,7 +8334,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B23" s="23" t="s">
         <v>51</v>
       </c>
@@ -8464,7 +8372,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B24" s="23" t="s">
         <v>47</v>
       </c>
@@ -8502,7 +8410,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B25" s="23" t="s">
         <v>58</v>
       </c>
@@ -8540,7 +8448,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B26" s="23" t="s">
         <v>44</v>
       </c>
@@ -8578,7 +8486,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B27" s="23" t="s">
         <v>68</v>
       </c>
@@ -8616,7 +8524,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B28" s="23" t="s">
         <v>46</v>
       </c>
@@ -8654,7 +8562,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B29" s="23" t="s">
         <v>49</v>
       </c>
@@ -8692,7 +8600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B30" s="23" t="s">
         <v>54</v>
       </c>
@@ -8730,7 +8638,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B31" s="23" t="s">
         <v>59</v>
       </c>
@@ -8768,7 +8676,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="B32" s="25"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -9018,15 +8926,15 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="13" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="13" width="16.453125" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="19"/>
@@ -9040,7 +8948,7 @@
       <c r="M1" s="19"/>
       <c r="N1" s="19"/>
     </row>
-    <row r="2" spans="1:14" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="37" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="22" t="s">
         <v>28</v>
@@ -9079,7 +8987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B3" s="23" t="s">
         <v>67</v>
       </c>
@@ -9117,7 +9025,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B4" s="23" t="s">
         <v>53</v>
       </c>
@@ -9155,7 +9063,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B5" s="23" t="s">
         <v>66</v>
       </c>
@@ -9193,7 +9101,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B6" s="23" t="s">
         <v>63</v>
       </c>
@@ -9231,7 +9139,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B7" s="23" t="s">
         <v>45</v>
       </c>
@@ -9269,7 +9177,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B8" s="23" t="s">
         <v>60</v>
       </c>
@@ -9307,7 +9215,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B9" s="23" t="s">
         <v>50</v>
       </c>
@@ -9345,7 +9253,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B10" s="23" t="s">
         <v>48</v>
       </c>
@@ -9383,7 +9291,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B11" s="23" t="s">
         <v>57</v>
       </c>
@@ -9421,7 +9329,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B12" s="23" t="s">
         <v>65</v>
       </c>
@@ -9459,7 +9367,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B13" s="23" t="s">
         <v>43</v>
       </c>
@@ -9497,7 +9405,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B14" s="23" t="s">
         <v>62</v>
       </c>
@@ -9535,7 +9443,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B15" s="23" t="s">
         <v>61</v>
       </c>
@@ -9573,7 +9481,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B16" s="23" t="s">
         <v>64</v>
       </c>
@@ -9611,7 +9519,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B17" s="23" t="s">
         <v>40</v>
       </c>
@@ -9649,7 +9557,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B18" s="23" t="s">
         <v>55</v>
       </c>
@@ -9687,7 +9595,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B19" s="23" t="s">
         <v>41</v>
       </c>
@@ -9725,7 +9633,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B20" s="23" t="s">
         <v>56</v>
       </c>
@@ -9763,7 +9671,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B21" s="23" t="s">
         <v>42</v>
       </c>
@@ -9801,7 +9709,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B22" s="23" t="s">
         <v>52</v>
       </c>
@@ -9839,7 +9747,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B23" s="23" t="s">
         <v>51</v>
       </c>
@@ -9877,7 +9785,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B24" s="23" t="s">
         <v>47</v>
       </c>
@@ -9915,7 +9823,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B25" s="23" t="s">
         <v>58</v>
       </c>
@@ -9953,7 +9861,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B26" s="23" t="s">
         <v>44</v>
       </c>
@@ -9991,7 +9899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B27" s="23" t="s">
         <v>68</v>
       </c>
@@ -10029,7 +9937,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B28" s="23" t="s">
         <v>46</v>
       </c>
@@ -10067,7 +9975,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B29" s="23" t="s">
         <v>49</v>
       </c>
@@ -10105,7 +10013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B30" s="23" t="s">
         <v>54</v>
       </c>
@@ -10143,7 +10051,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B31" s="23" t="s">
         <v>59</v>
       </c>
@@ -10181,7 +10089,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" ht="18.5" x14ac:dyDescent="0.35">
       <c r="B32" s="25"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -10243,6 +10151,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D31">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{67855C88-1405-410A-A886-7BC1495DEEBD}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
@@ -10252,18 +10172,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{E5B03E62-9AA2-46B7-AB1E-87B49F690041}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="20">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{67855C88-1405-410A-A886-7BC1495DEEBD}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10279,6 +10187,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E31">
+    <cfRule type="dataBar" priority="18">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{A141A3A9-B5D3-4F6B-8ECA-B4BD5B0A3E81}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="min"/>
@@ -10288,18 +10208,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{F5DED1AF-6C55-4C76-AA18-F01EF9A870AE}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="18">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{A141A3A9-B5D3-4F6B-8ECA-B4BD5B0A3E81}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10315,6 +10223,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F31">
+    <cfRule type="dataBar" priority="16">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{03E1D33C-812B-4932-8E25-8CCE7881A196}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="min"/>
@@ -10324,18 +10244,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{3559B80D-FD21-4FDE-914C-B8DB9CA58C0A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="16">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{03E1D33C-812B-4932-8E25-8CCE7881A196}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10351,6 +10259,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G31">
+    <cfRule type="dataBar" priority="14">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D966ADC9-B0C4-4674-9C20-E4C31EC1A986}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="min"/>
@@ -10360,18 +10280,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{63D820D7-954E-41E6-A526-DFB26DD88B4E}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="14">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D966ADC9-B0C4-4674-9C20-E4C31EC1A986}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10387,6 +10295,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3:H31">
+    <cfRule type="dataBar" priority="12">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B2EC3799-C5E5-499F-BD55-997115519953}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="11">
       <dataBar>
         <cfvo type="min"/>
@@ -10396,18 +10316,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{679A18B5-8F27-4735-B81B-4E702F8DF44A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="12">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{B2EC3799-C5E5-499F-BD55-997115519953}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10567,6 +10475,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M31">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3985B7E6-92A8-43A1-96A7-CA3104060C8D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -10576,18 +10496,6 @@
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
           <x14:id>{BD10008D-318B-4307-81F1-78CE7347670A}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-    <cfRule type="dataBar" priority="2">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF555A"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{3985B7E6-92A8-43A1-96A7-CA3104060C8D}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -10620,6 +10528,16 @@
           <xm:sqref>C3:C31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{67855C88-1405-410A-A886-7BC1495DEEBD}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
           <x14:cfRule type="dataBar" id="{E5B03E62-9AA2-46B7-AB1E-87B49F690041}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="min"/>
@@ -10630,7 +10548,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{67855C88-1405-410A-A886-7BC1495DEEBD}">
+          <xm:sqref>D3:D31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{A141A3A9-B5D3-4F6B-8ECA-B4BD5B0A3E81}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10640,9 +10561,6 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D3:D31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F5DED1AF-6C55-4C76-AA18-F01EF9A870AE}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="min"/>
@@ -10653,7 +10571,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{A141A3A9-B5D3-4F6B-8ECA-B4BD5B0A3E81}">
+          <xm:sqref>E3:E31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{03E1D33C-812B-4932-8E25-8CCE7881A196}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10663,9 +10584,6 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E3:E31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{3559B80D-FD21-4FDE-914C-B8DB9CA58C0A}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="min"/>
@@ -10676,7 +10594,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{03E1D33C-812B-4932-8E25-8CCE7881A196}">
+          <xm:sqref>F3:F31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D966ADC9-B0C4-4674-9C20-E4C31EC1A986}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10686,9 +10607,6 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F3:F31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{63D820D7-954E-41E6-A526-DFB26DD88B4E}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="min"/>
@@ -10699,7 +10617,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{D966ADC9-B0C4-4674-9C20-E4C31EC1A986}">
+          <xm:sqref>G3:G31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B2EC3799-C5E5-499F-BD55-997115519953}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="autoMin"/>
               <x14:cfvo type="autoMax"/>
@@ -10709,23 +10630,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>G3:G31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{679A18B5-8F27-4735-B81B-4E702F8DF44A}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
               <x14:cfvo type="min"/>
               <x14:cfvo type="max"/>
-              <x14:borderColor rgb="FFFF555A"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{B2EC3799-C5E5-499F-BD55-997115519953}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
               <x14:borderColor rgb="FFFF555A"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:negativeBorderColor rgb="FFFF0000"/>
@@ -10827,20 +10735,20 @@
           <xm:sqref>L3:L31</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BD10008D-318B-4307-81F1-78CE7347670A}">
+          <x14:cfRule type="dataBar" id="{3985B7E6-92A8-43A1-96A7-CA3104060C8D}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="min"/>
-              <x14:cfvo type="max"/>
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
               <x14:borderColor rgb="FFFF555A"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:negativeBorderColor rgb="FFFF0000"/>
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <x14:cfRule type="dataBar" id="{3985B7E6-92A8-43A1-96A7-CA3104060C8D}">
+          <x14:cfRule type="dataBar" id="{BD10008D-318B-4307-81F1-78CE7347670A}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
+              <x14:cfvo type="min"/>
+              <x14:cfvo type="max"/>
               <x14:borderColor rgb="FFFF555A"/>
               <x14:negativeFillColor rgb="FFFF0000"/>
               <x14:negativeBorderColor rgb="FFFF0000"/>
@@ -10857,74 +10765,73 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A2A028-B814-4548-AC54-3A238B244BD7}">
-  <dimension ref="B3:E6"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.7265625" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="47">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="54">
         <v>7</v>
       </c>
-      <c r="C3">
-        <v>56</v>
-      </c>
-      <c r="D3" s="47">
-        <v>9</v>
-      </c>
-      <c r="E3">
+      <c r="C3" s="53">
+        <v>66</v>
+      </c>
+      <c r="D3" s="54">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="47">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="54">
         <v>15</v>
       </c>
-      <c r="C4">
-        <v>22</v>
-      </c>
-      <c r="D4" s="47">
-        <v>17</v>
-      </c>
-      <c r="E4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="47">
+      <c r="C4" s="53">
+        <v>32</v>
+      </c>
+      <c r="D4" s="54">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="54">
         <v>54</v>
       </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5" s="47">
-        <v>59</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="53">
+        <v>40</v>
+      </c>
+      <c r="D5" s="54">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="54">
+        <v>5</v>
+      </c>
+      <c r="C6" s="53">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="47">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>25</v>
-      </c>
-      <c r="D6" s="47">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>15</v>
+      <c r="D6" s="54">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>